<commit_message>
adding changes as on 3sept24
</commit_message>
<xml_diff>
--- a/stack/IP_DATA/IP_DATA.xlsx
+++ b/stack/IP_DATA/IP_DATA.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC70068\eclipse-workspace\SBA\stack\IP_DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC70068\git\ServiceCleanup\stack\IP_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A52650-05BB-4006-AD28-E17250A339CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25AB484-DE4A-45AE-B638-2861F4D66CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Credentials" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>CircuitID</t>
   </si>
@@ -35,22 +47,116 @@
   </si>
   <si>
     <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>InventoryType</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>ACT Cleanup WorkFlow</t>
+  </si>
+  <si>
+    <t>InventoryOnlyCleanup</t>
+  </si>
+  <si>
+    <t>ASRI</t>
+  </si>
+  <si>
+    <t>RobVanDam@wwf@1992#</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>AC70068</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060533/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060512/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060515/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060529/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060532/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060516/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060537/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060547/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060540/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060548/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060541/LUMN</t>
+  </si>
+  <si>
+    <t>IL/IRXX/066021/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060549/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060542/LUMN</t>
+  </si>
+  <si>
+    <t>IL/IRXX/066019/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060507/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060497/LUMN</t>
+  </si>
+  <si>
+    <t>CO/IRXX/060508/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060543/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060511/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060493/LUMN</t>
+  </si>
+  <si>
+    <t>VA/IRXX/060544/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060498/LUMN</t>
+  </si>
+  <si>
+    <t>TX/IRXX/060494/LUMN</t>
+  </si>
+  <si>
+    <t>CleanIP_Using_Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,6 +170,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -80,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -103,17 +230,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,23 +572,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{C54D6153-C93A-4784-90E0-3B83EC1B6D15}">
+      <formula1>" ,TEST1,TEST2,TEST4"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{3C34DB73-1D7C-4D7F-8531-9D7663AEC76F}">
+      <formula1>"DELETE,DEACTIVATE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{45ED2C24-2C28-4BE9-9519-37DF6DE165A1}">
+      <formula1>"ASRI,ARM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{57E5F9DB-9445-4426-A9B4-7A1437A2DA96}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -416,31 +645,301 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18539128-BE31-4DFF-BED5-88E1400B7634}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C6B788E-DAE9-41F0-9BE3-AD14778F3FE5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8164E1-5980-42C2-B380-ECE8FFC75733}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9">
+        <v>7763020093</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="9">
+        <v>7763020902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9">
+        <v>7763028199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9">
+        <v>7763028199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9">
+        <v>7763029202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9">
+        <v>7763029215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9">
+        <v>7763029502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7763030806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7763031417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="9">
+        <v>7763031440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9">
+        <v>7763031553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9">
+        <v>7763031745</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="9">
+        <v>7763032029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="9">
+        <v>7763033847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="9">
+        <v>7763036616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="9">
+        <v>7763036915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="9">
+        <v>7763037179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="9">
+        <v>7763037197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="9">
+        <v>7763037518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="9">
+        <v>7763038874</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9">
+        <v>7763038898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="9">
+        <v>7763039159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="9">
+        <v>7763040445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="9">
+        <v>7763041091</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D25" s="9">
+        <v>7763041807</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D26" s="9">
+        <v>7763042479</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D27" s="9">
+        <v>7763042643</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D28" s="9">
+        <v>7763044268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D29" s="9">
+        <v>7763044498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D30" s="9">
+        <v>7763044651</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D31" s="9">
+        <v>7763044873</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D32" s="9">
+        <v>7763044885</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" s="9">
+        <v>7763044940</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f7bd1f64-4ecb-43d7-94b5-4669091ae21c}" enabled="1" method="Privileged" siteId="{72b17115-9915-42c0-9f1b-4f98e5a4bcd2}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>